<commit_message>
feat: agora nesse ponto está salvando o excel com os dados da struct, ou seja, cada atributo é a coluna, caso o valor do atributo seja maior que 1 ele atribui um dropdown.
</commit_message>
<xml_diff>
--- a/exemple-export-template-excel/example.xlsx
+++ b/exemple-export-template-excel/example.xlsx
@@ -14,15 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Número</t>
+    <t>Name</t>
   </si>
   <si>
-    <t>Mês</t>
+    <t>Age</t>
   </si>
   <si>
-    <t>Ano</t>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Games</t>
   </si>
 </sst>
 </file>
@@ -341,14 +344,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation allowBlank="true" sqref="B2:B1000" type="list">
-      <formula1>"Janeiro,Fevereiro,Março,Abril,Maio,Junho,Julho,Agosto,Setembro,Outubro,Novembro,Dezembro"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="true" sqref="C2:C1000" type="list">
-      <formula1>"2010,2011,2012,2013,2014,2015,2016,2017,2018,2019,2020,2021,2022,2023,2024,2025,2026,2027,2028,2029,2030"</formula1>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" sqref="D2:D100000" type="list">
+      <formula1>"Super Mario,SONIC,Zelda,GTA"</formula1>
     </dataValidation>
   </dataValidations>
 </worksheet>

</xml_diff>

<commit_message>
feat: finalizado o teste de geração de templates para preenchimento usando dropdowns.
</commit_message>
<xml_diff>
--- a/exemple-export-template-excel/example.xlsx
+++ b/exemple-export-template-excel/example.xlsx
@@ -16,16 +16,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Games</t>
+  </si>
+  <si>
     <t>Name</t>
   </si>
   <si>
     <t>Age</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Games</t>
   </si>
 </sst>
 </file>
@@ -350,7 +350,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" sqref="D2:D100000" type="list">
+    <dataValidation allowBlank="true" sqref="B2:B100000" type="list">
       <formula1>"Super Mario,SONIC,Zelda,GTA"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>